<commit_message>
Update the email to a valid one in excel: US9414_03.xlsx
</commit_message>
<xml_diff>
--- a/data/US9414_03.xlsx
+++ b/data/US9414_03.xlsx
@@ -42,7 +42,7 @@
     <t>Encore CSR Group</t>
   </si>
   <si>
-    <t>jahaziel.rosales@hpe.com</t>
+    <t>yu.li9@hpe.com</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -420,11 +420,17 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>